<commit_message>
need to insert facs data and after implement unique forms for users
</commit_message>
<xml_diff>
--- a/DB_Setup.xlsx
+++ b/DB_Setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\FACULTATE\LICENTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCEE1DF-CD4F-4C65-A283-3F12868A686E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55344F0-44EA-406F-9E4E-F728A19BCDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="15576" windowHeight="11904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Universitati</t>
   </si>
@@ -93,39 +93,6 @@
     <t>Users</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Tip user</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>elev</t>
-  </si>
-  <si>
-    <t>student</t>
-  </si>
-  <si>
-    <t>profesor</t>
-  </si>
-  <si>
-    <t>consilier cariera</t>
-  </si>
-  <si>
-    <t>ID_tipuser - PK</t>
-  </si>
-  <si>
-    <t>ID_tipuser - FK</t>
-  </si>
-  <si>
-    <t>tip_nume       =&gt;</t>
-  </si>
-  <si>
     <t>Intrebari Formular Elevi</t>
   </si>
   <si>
@@ -142,6 +109,18 @@
   </si>
   <si>
     <t>5. In ce oras v-ati dori sa fie facultatea?</t>
+  </si>
+  <si>
+    <t>username - PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tip </t>
+  </si>
+  <si>
+    <t>passwd</t>
+  </si>
+  <si>
+    <t>ID_fac - FK</t>
   </si>
 </sst>
 </file>
@@ -197,16 +176,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,33 +466,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="13" max="13" width="31.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -540,13 +517,13 @@
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -568,187 +545,151 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G7" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="J7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="3"/>
       <c r="M7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="M8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="3"/>
+      <c r="G9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="M9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C16" s="5" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="2"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" t="s">
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" t="s">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="G11:H16"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="G7:H7"/>
+  <mergeCells count="11">
     <mergeCell ref="G1:H3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="598" r:id="rId1"/>

</xml_diff>

<commit_message>
de facut add to favorites,paginare, admin
</commit_message>
<xml_diff>
--- a/DB_Setup.xlsx
+++ b/DB_Setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\FACULTATE\LICENTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ECA5DC-7FEA-413B-91B3-0B8D3D081DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1C56BA-71E8-4D34-8427-7F6A64FE55D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t>Universitati</t>
   </si>
@@ -228,6 +228,69 @@
   </si>
   <si>
     <t>În ce domenii ați dori să se încadreze facultățile afișate?</t>
+  </si>
+  <si>
+    <t>1. Facultatea de Automatică și Calculatoare:</t>
+  </si>
+  <si>
+    <t>Inovație și cercetare</t>
+  </si>
+  <si>
+    <t>Dezvoltarea abilităților practice</t>
+  </si>
+  <si>
+    <t>2. Facultatea de Electronică, Telecomunicații și Tehnologia Informației:</t>
+  </si>
+  <si>
+    <t>3. Facultatea de Energetică:</t>
+  </si>
+  <si>
+    <t>Contribuția socială</t>
+  </si>
+  <si>
+    <t>4. Facultatea de Inginerie Chimică și Protecția Mediului:</t>
+  </si>
+  <si>
+    <t>Sustenabilitate și responsabilitate socială</t>
+  </si>
+  <si>
+    <t>5. Facultatea de Inginerie Economică și Generală:</t>
+  </si>
+  <si>
+    <t>Dezvoltarea personală și profesională</t>
+  </si>
+  <si>
+    <t>6. Facultatea de Inginerie Mecanică și Mecatronică:</t>
+  </si>
+  <si>
+    <t>Abordarea interdisciplinară</t>
+  </si>
+  <si>
+    <t>7. Facultatea de Inginerie în Limbi Străine:</t>
+  </si>
+  <si>
+    <t>8. Facultatea de Inginerie și Management în Agricultură și Dezvoltare Rurală:</t>
+  </si>
+  <si>
+    <t>9. Facultatea de Inginerie și Management Industrial:</t>
+  </si>
+  <si>
+    <t>Leadership și management</t>
+  </si>
+  <si>
+    <t>10. Facultatea de Metrologie, Calitate și Management:</t>
+  </si>
+  <si>
+    <t>11. Facultatea de Telecomunicații:</t>
+  </si>
+  <si>
+    <t>12. Facultatea de Textile și Pielărie:</t>
+  </si>
+  <si>
+    <t>Creativitate și exprimare artistică</t>
+  </si>
+  <si>
+    <t>13. Facultatea de Transporturi:</t>
   </si>
 </sst>
 </file>
@@ -320,12 +383,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -608,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N79"/>
+  <dimension ref="A1:N146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:D46"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,16 +688,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -652,20 +715,20 @@
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="M4" s="10" t="s">
+      <c r="K4" s="11"/>
+      <c r="M4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="10"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -677,27 +740,27 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="J6" s="11" t="s">
+      <c r="H6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="9"/>
       <c r="M6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="J7" s="11" t="s">
+      <c r="H7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="11"/>
+      <c r="K7" s="9"/>
       <c r="M7" t="s">
         <v>17</v>
       </c>
@@ -712,8 +775,8 @@
       <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
       <c r="M8" t="s">
         <v>7</v>
       </c>
@@ -728,8 +791,8 @@
       <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
       <c r="M9" t="s">
         <v>15</v>
       </c>
@@ -849,11 +912,11 @@
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
       <c r="F36" s="4" t="s">
         <v>37</v>
       </c>
@@ -861,22 +924,22 @@
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="4"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
       <c r="F38" s="6" t="s">
         <v>38</v>
       </c>
@@ -884,12 +947,12 @@
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
       <c r="F39" s="4" t="s">
         <v>39</v>
       </c>
@@ -919,19 +982,19 @@
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
       <c r="F43" s="4"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
       <c r="F44" s="6" t="s">
         <v>34</v>
       </c>
@@ -939,11 +1002,11 @@
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
       <c r="F45" s="4" t="s">
         <v>41</v>
       </c>
@@ -951,17 +1014,17 @@
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
       <c r="F47" s="6" t="s">
         <v>38</v>
       </c>
@@ -969,9 +1032,9 @@
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
       <c r="F48" s="4" t="s">
         <v>42</v>
       </c>
@@ -979,9 +1042,9 @@
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
@@ -1095,15 +1158,249 @@
         <v>59</v>
       </c>
     </row>
+    <row r="95" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B96" s="4"/>
+    </row>
+    <row r="97" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B97" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B98" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B100" s="4"/>
+    </row>
+    <row r="101" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B101" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B102" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B104" s="4"/>
+    </row>
+    <row r="105" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B105" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B106" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B108" s="4"/>
+    </row>
+    <row r="109" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B109" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B110" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B112" s="4"/>
+    </row>
+    <row r="113" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B113" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B114" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+    </row>
+    <row r="117" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B117" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B118" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+    </row>
+    <row r="121" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B121" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B122" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B124" s="4"/>
+    </row>
+    <row r="125" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B125" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B126" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B128" s="4"/>
+    </row>
+    <row r="129" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B129" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B130" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B132" s="4"/>
+    </row>
+    <row r="133" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B133" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B134" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B136" s="4"/>
+    </row>
+    <row r="137" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B137" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B138" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B140" s="4"/>
+    </row>
+    <row r="141" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B141" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B142" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B144" s="4"/>
+    </row>
+    <row r="145" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B145" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B146" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="G1:H3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
@@ -1112,13 +1409,13 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="598" r:id="rId1"/>

</xml_diff>